<commit_message>
cleaned version of assignment
</commit_message>
<xml_diff>
--- a/6. Coding and documentation/Data/Eurostat_employment_isco.xlsx
+++ b/6. Coding and documentation/Data/Eurostat_employment_isco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whard\OneDrive\Desktop\Reproducible research\Recoding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkalisiak003\Desktop\ReproducibleResearch\RRcourse2023\6. Coding and documentation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BEFDF46-A361-48D8-9834-62D13AAA7D9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A29874-0CD8-43BC-8359-46D09492F1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21732" windowHeight="5940" xr2:uid="{AB8E089C-3C03-4BA6-B14E-D8632E128822}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{AB8E089C-3C03-4BA6-B14E-D8632E128822}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,9 +333,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,7 +373,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -479,7 +479,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -631,13 +631,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38363672-59F0-4595-8DCF-6E865AA04F3A}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -707,7 +707,7 @@
         <v>4406.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -742,7 +742,7 @@
         <v>4519.3999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -777,7 +777,7 @@
         <v>4578.8999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -812,7 +812,7 @@
         <v>4487.8999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -847,7 +847,7 @@
         <v>4428.3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -882,7 +882,7 @@
         <v>4531.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -917,7 +917,7 @@
         <v>4585</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -952,7 +952,7 @@
         <v>4493.7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -987,7 +987,7 @@
         <v>4460.2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>4564.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>4637.6000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>4554.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>4499.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>4603.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>4698.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>4588.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>4559.3999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>4658.8999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>4744.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>4676.8999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>4638</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>4755.3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>4806.3999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>4742.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>4745.1000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>4842.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>4912.8</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>4834.8999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>4823.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>4928.8999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>4985.1000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>4903.3999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>4864.2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>4954.8999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>5006</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>4928.8999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>4849.3999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>4846.3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>4897.1000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -2082,12 +2082,12 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>220.6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>240.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>244.8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>231.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>235.4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>239.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>223.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>222.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>234.8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>237.1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>224.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>234.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>251.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>226.4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>221.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>237.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>230.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>218.6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>228.1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>239.9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>231.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>230.4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>230.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>238.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>224.9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>221.1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>237.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>226.9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>238.7</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>217.4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>217.5</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>210.3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -3535,9 +3535,9 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>238.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>246.1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>249.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>260.7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>266.10000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>265.60000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>265.39999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>257.3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>265.10000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>261.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>260.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>257.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>254.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>251.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>253.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>260.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>270.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>267.89999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>290.60000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>279.60000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>284.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>286.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>288.7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>299.10000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>302.89999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>297.7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>310.5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>300.39999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>313.7</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>315.39999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>312.89999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>309.5</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>311.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -4985,9 +4985,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>1102.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>1125.4000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>1131.2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>1135.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>1135.5999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>1127.7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>1144.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>1144.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>1161.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>1160.5999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>1193.3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>1202.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>1217.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>1222.5999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>1237.5999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>1248.5999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>1261.4000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>1276.4000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>1314.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>1325.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>1327.2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>1325.9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>1342.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>1351.9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>1362.6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>1408.9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>1424.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>1421.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>1445.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>1471.2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>1475.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>1489.4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>1502.2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>1495.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -6435,9 +6435,9 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>722.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>722.3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>730.2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>733.9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>731.7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>740.9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>745.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>760.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>762.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>775.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>779.8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>788.2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>793.7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>805.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>818.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>812.3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>831.9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>828.8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>831.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>843.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>858.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>862.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>858.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>855.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>871.2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>902.2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>891.6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>902.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>913.9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>914.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>908.4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>904.7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>897.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>907.3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>927.8</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>922.2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>904.8</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>923.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -7885,9 +7885,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>267.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>275.10000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>271.89999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>261.10000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>268.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>261.3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>273.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>279.2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>267.39999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -8377,7 +8377,7 @@
         <v>261.60000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>273.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>291.89999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>276.60000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -8517,7 +8517,7 @@
         <v>277.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>290.10000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>310.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>308.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>302.60000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>300.60000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>304.39999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -8762,7 +8762,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>299.10000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>315.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -8867,7 +8867,7 @@
         <v>322.60000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>309.39999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>310.8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>307.7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>313.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>287.5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>287.89999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>293.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -9182,7 +9182,7 @@
         <v>294.2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>269.39999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -9252,7 +9252,7 @@
         <v>282.7</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>291.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -9329,16 +9329,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA20AC9-EAA9-43DD-8DD7-3B4A74C3BB15}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9373,7 +9372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -9408,7 +9407,7 @@
         <v>920.7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -9443,7 +9442,7 @@
         <v>956.6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -9478,7 +9477,7 @@
         <v>984.3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -9513,7 +9512,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -9548,7 +9547,7 @@
         <v>916.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -9583,7 +9582,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -9618,7 +9617,7 @@
         <v>976.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -9653,7 +9652,7 @@
         <v>916.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -9688,7 +9687,7 @@
         <v>908.4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -9723,7 +9722,7 @@
         <v>938.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -9758,7 +9757,7 @@
         <v>966.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -9793,7 +9792,7 @@
         <v>919.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -9828,7 +9827,7 @@
         <v>908.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -9863,7 +9862,7 @@
         <v>932.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -9898,7 +9897,7 @@
         <v>971.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -9933,7 +9932,7 @@
         <v>919.7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -9968,7 +9967,7 @@
         <v>899.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -10003,7 +10002,7 @@
         <v>940.3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -10038,7 +10037,7 @@
         <v>962.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -10073,7 +10072,7 @@
         <v>905.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -10108,7 +10107,7 @@
         <v>889.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -10143,7 +10142,7 @@
         <v>933.3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -10178,7 +10177,7 @@
         <v>940.6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -10213,7 +10212,7 @@
         <v>920.9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -10248,7 +10247,7 @@
         <v>918.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -10283,7 +10282,7 @@
         <v>952.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -10318,7 +10317,7 @@
         <v>964.3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -10353,7 +10352,7 @@
         <v>932.7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -10388,7 +10387,7 @@
         <v>901.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -10423,7 +10422,7 @@
         <v>930.8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -10458,7 +10457,7 @@
         <v>940.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -10493,7 +10492,7 @@
         <v>890.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -10528,7 +10527,7 @@
         <v>885.7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -10563,7 +10562,7 @@
         <v>917.6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -10598,7 +10597,7 @@
         <v>925.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -10633,7 +10632,7 @@
         <v>879.7</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -10668,7 +10667,7 @@
         <v>857.3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -10703,7 +10702,7 @@
         <v>845.9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -10738,7 +10737,7 @@
         <v>854.7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -10774,11 +10773,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K41" xr:uid="{8C5CB4E7-3900-4EC4-AFC5-84CDEE4C2434}">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10791,9 +10785,9 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10828,7 +10822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -10863,7 +10857,7 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -10898,7 +10892,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -10933,7 +10927,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -10968,7 +10962,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -11003,7 +10997,7 @@
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -11038,7 +11032,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -11073,7 +11067,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -11108,7 +11102,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -11143,7 +11137,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -11178,7 +11172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -11213,7 +11207,7 @@
         <v>77.3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -11248,7 +11242,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -11283,7 +11277,7 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -11318,7 +11312,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -11353,7 +11347,7 @@
         <v>78.3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -11388,7 +11382,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -11423,7 +11417,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -11458,7 +11452,7 @@
         <v>77.400000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -11493,7 +11487,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -11528,7 +11522,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -11563,7 +11557,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -11598,7 +11592,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -11633,7 +11627,7 @@
         <v>79.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -11668,7 +11662,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -11703,7 +11697,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -11738,7 +11732,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -11773,7 +11767,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -11808,7 +11802,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -11843,7 +11837,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -11878,7 +11872,7 @@
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -11913,7 +11907,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -11948,7 +11942,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -11983,7 +11977,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -12018,7 +12012,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -12053,7 +12047,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -12088,7 +12082,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -12123,7 +12117,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -12158,7 +12152,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -12193,7 +12187,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -12241,9 +12235,9 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12278,7 +12272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -12313,7 +12307,7 @@
         <v>474.4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -12348,7 +12342,7 @@
         <v>495.9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -12383,7 +12377,7 @@
         <v>501.3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -12418,7 +12412,7 @@
         <v>491.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -12453,7 +12447,7 @@
         <v>468.6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -12488,7 +12482,7 @@
         <v>474.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -12523,7 +12517,7 @@
         <v>479.6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -12558,7 +12552,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -12593,7 +12587,7 @@
         <v>447.7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -12628,7 +12622,7 @@
         <v>456.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -12663,7 +12657,7 @@
         <v>466.8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -12698,7 +12692,7 @@
         <v>453.1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -12733,7 +12727,7 @@
         <v>440.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -12768,7 +12762,7 @@
         <v>452.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -12803,7 +12797,7 @@
         <v>451.1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -12838,7 +12832,7 @@
         <v>450.9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -12873,7 +12867,7 @@
         <v>431.6</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -12908,7 +12902,7 @@
         <v>452.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -12943,7 +12937,7 @@
         <v>462.6</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -12978,7 +12972,7 @@
         <v>453.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -13013,7 +13007,7 @@
         <v>438.1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -13048,7 +13042,7 @@
         <v>443.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -13083,7 +13077,7 @@
         <v>448.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -13118,7 +13112,7 @@
         <v>447.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -13153,7 +13147,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -13188,7 +13182,7 @@
         <v>451.6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -13223,7 +13217,7 @@
         <v>456.3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -13258,7 +13252,7 @@
         <v>447.7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -13293,7 +13287,7 @@
         <v>449.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -13328,7 +13322,7 @@
         <v>455.1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -13363,7 +13357,7 @@
         <v>457.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -13398,7 +13392,7 @@
         <v>453.7</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -13433,7 +13427,7 @@
         <v>464.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -13468,7 +13462,7 @@
         <v>459.2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -13503,7 +13497,7 @@
         <v>467.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -13538,7 +13532,7 @@
         <v>446.6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -13573,7 +13567,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -13608,7 +13602,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -13643,7 +13637,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
@@ -13691,9 +13685,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13728,7 +13722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -13763,7 +13757,7 @@
         <v>362.2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -13798,7 +13792,7 @@
         <v>369.1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -13833,7 +13827,7 @@
         <v>373.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -13868,7 +13862,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -13903,7 +13897,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -13938,7 +13932,7 @@
         <v>352.3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -13973,7 +13967,7 @@
         <v>366.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -14008,7 +14002,7 @@
         <v>345.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -14043,7 +14037,7 @@
         <v>339.9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
@@ -14078,7 +14072,7 @@
         <v>357.8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -14113,7 +14107,7 @@
         <v>356.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -14148,7 +14142,7 @@
         <v>347.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -14183,7 +14177,7 @@
         <v>338.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -14218,7 +14212,7 @@
         <v>346.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -14253,7 +14247,7 @@
         <v>345.9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
@@ -14288,7 +14282,7 @@
         <v>334.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
@@ -14323,7 +14317,7 @@
         <v>327.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
@@ -14358,7 +14352,7 @@
         <v>319.3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -14393,7 +14387,7 @@
         <v>320.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -14428,7 +14422,7 @@
         <v>307.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -14463,7 +14457,7 @@
         <v>293.89999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -14498,7 +14492,7 @@
         <v>299.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -14533,7 +14527,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -14568,7 +14562,7 @@
         <v>283.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -14603,7 +14597,7 @@
         <v>285.89999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -14638,7 +14632,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -14673,7 +14667,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -14708,7 +14702,7 @@
         <v>281.10000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -14743,7 +14737,7 @@
         <v>278.2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -14778,7 +14772,7 @@
         <v>281.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -14813,7 +14807,7 @@
         <v>294.39999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -14848,7 +14842,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>43</v>
       </c>
@@ -14883,7 +14877,7 @@
         <v>275.3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -14918,7 +14912,7 @@
         <v>287.3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -14953,7 +14947,7 @@
         <v>293.60000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -14988,7 +14982,7 @@
         <v>269.8</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -15023,7 +15017,7 @@
         <v>272.2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
@@ -15058,7 +15052,7 @@
         <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
@@ -15093,7 +15087,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>51</v>
       </c>

</xml_diff>